<commit_message>
Tabela atualizada com Timestamp e CurrentNode
</commit_message>
<xml_diff>
--- a/hempsMPEG.xlsx
+++ b/hempsMPEG.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="8">
   <si>
     <t>Header</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>Target</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>CurrentNode</t>
   </si>
 </sst>
 </file>
@@ -408,19 +414,21 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F2208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>

</xml_diff>